<commit_message>
Updates Forms C & D
</commit_message>
<xml_diff>
--- a/ILRG_ORAM_C_limites/ILRG_ORAM_C_limites-media/ILRG_ORAM_C_limites.xlsx
+++ b/ILRG_ORAM_C_limites/ILRG_ORAM_C_limites-media/ILRG_ORAM_C_limites.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\projects\ILRG\Grants\Dams project\ODK Forms\ILRG_ORAM_odk_forms\ILRG_ORAM_C_limites\ILRG_ORAM_C_limites-media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC44D6A-3973-48D0-BF73-4524D07D009E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33320113-ED37-4E8D-826E-0C4C2186D52A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13740" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -3352,9 +3352,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -3566,385 +3573,386 @@
   </borders>
   <cellStyleXfs count="238">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="237" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="237" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="237" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="237" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="237" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="237"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="233" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="234" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="234" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="237" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="237" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="235" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="237" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="237" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="237" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="237"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="233" applyFont="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="234" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="234" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="235" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="238">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -4523,11 +4531,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C33" sqref="C33"/>
+      <selection pane="bottomRight" activeCell="B17" sqref="B17:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4623,7 +4631,7 @@
       <c r="B5" s="29" t="s">
         <v>1031</v>
       </c>
-      <c r="M5" s="56" t="s">
+      <c r="M5" s="66" t="s">
         <v>1048</v>
       </c>
     </row>
@@ -4687,7 +4695,7 @@
       <c r="B11" s="57" t="s">
         <v>1072</v>
       </c>
-      <c r="C11" s="64" t="s">
+      <c r="C11" s="66" t="s">
         <v>1103</v>
       </c>
       <c r="J11" s="13" t="s">
@@ -4953,7 +4961,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5260,9 +5268,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F4195"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A520" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C542" sqref="C542"/>
+      <selection pane="bottomLeft" activeCell="C545" sqref="C545"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30544,7 +30552,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>